<commit_message>
updated trunk to latest 2.2.x
</commit_message>
<xml_diff>
--- a/iRINGTools.Services/App_Data/Equipment.xlsx
+++ b/iRINGTools.Services/App_Data/Equipment.xlsx
@@ -1,99 +1,236 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<x:workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <x:fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
-  <x:workbookPr defaultThemeVersion="124226"/>
-  <x:bookViews>
-    <x:workbookView xWindow="0" yWindow="135" windowWidth="23955" windowHeight="9780"/>
-  </x:bookViews>
-  <x:sheets>
-    <x:sheet name="Equipment" sheetId="1" r:id="rId1"/>
-  </x:sheets>
-  <x:calcPr calcId="125725"/>
-</x:workbook>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <workbookPr defaultThemeVersion="124226"/>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="135" windowWidth="23955" windowHeight="9780" activeTab="1"/>
+  </bookViews>
+  <sheets>
+    <sheet name="Equipment" sheetId="1" r:id="rId1"/>
+    <sheet name="Lines" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
+  </sheets>
+  <calcPr calcId="125725"/>
+</workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="26">
-  <x:si>
-    <x:t>Equip-005</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Equip-006</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Equip-007</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Equip-008</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Tag</x:t>
-  </x:si>
-  <x:si>
-    <x:t>PumpType</x:t>
-  </x:si>
-  <x:si>
-    <x:t>PumpDriverType</x:t>
-  </x:si>
-  <x:si>
-    <x:t>DesignTemp</x:t>
-  </x:si>
-  <x:si>
-    <x:t>DesignPressure</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Capacity</x:t>
-  </x:si>
-  <x:si>
-    <x:t>SpecificGravity</x:t>
-  </x:si>
-  <x:si>
-    <x:t>DifferentialPressure</x:t>
-  </x:si>
-  <x:si>
-    <x:t>PT-5</x:t>
-  </x:si>
-  <x:si>
-    <x:t>PDT-6</x:t>
-  </x:si>
-  <x:si>
-    <x:t>PDT-8</x:t>
-  </x:si>
-  <x:si>
-    <x:t>PDT-3</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Equip-001</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Equip-002</x:t>
-  </x:si>
-  <x:si>
-    <x:t>PT-7</x:t>
-  </x:si>
-  <x:si>
-    <x:t>PDT-5</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Equip-003</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Equip-004</x:t>
-  </x:si>
-  <x:si>
-    <x:t>PT-3</x:t>
-  </x:si>
-  <x:si>
-    <x:t>PDT-4</x:t>
-  </x:si>
-  <x:si>
-    <x:t>PDT-7</x:t>
-  </x:si>
-  <x:si>
-    <x:t>PT-4</x:t>
-  </x:si>
-</x:sst>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="71">
+  <si>
+    <t>Equip-005</t>
+  </si>
+  <si>
+    <t>Equip-006</t>
+  </si>
+  <si>
+    <t>Equip-007</t>
+  </si>
+  <si>
+    <t>Equip-008</t>
+  </si>
+  <si>
+    <t>Tag</t>
+  </si>
+  <si>
+    <t>PumpType</t>
+  </si>
+  <si>
+    <t>PumpDriverType</t>
+  </si>
+  <si>
+    <t>DesignTemp</t>
+  </si>
+  <si>
+    <t>DesignPressure</t>
+  </si>
+  <si>
+    <t>Capacity</t>
+  </si>
+  <si>
+    <t>SpecificGravity</t>
+  </si>
+  <si>
+    <t>DifferentialPressure</t>
+  </si>
+  <si>
+    <t>PT-5</t>
+  </si>
+  <si>
+    <t>PDT-6</t>
+  </si>
+  <si>
+    <t>PDT-8</t>
+  </si>
+  <si>
+    <t>PDT-3</t>
+  </si>
+  <si>
+    <t>Equip-001</t>
+  </si>
+  <si>
+    <t>Equip-002</t>
+  </si>
+  <si>
+    <t>PT-7</t>
+  </si>
+  <si>
+    <t>PDT-5</t>
+  </si>
+  <si>
+    <t>Equip-003</t>
+  </si>
+  <si>
+    <t>Equip-004</t>
+  </si>
+  <si>
+    <t>PT-3</t>
+  </si>
+  <si>
+    <t>PDT-4</t>
+  </si>
+  <si>
+    <t>PT-8</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>PDT-9</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>PT-6</t>
+  </si>
+  <si>
+    <t>SystenNumber</t>
+  </si>
+  <si>
+    <t>LineNumber</t>
+  </si>
+  <si>
+    <t>AreaNumber</t>
+  </si>
+  <si>
+    <t>TAG001</t>
+  </si>
+  <si>
+    <t>TAG002</t>
+  </si>
+  <si>
+    <t>TAG003</t>
+  </si>
+  <si>
+    <t>TAG004</t>
+  </si>
+  <si>
+    <t>TAG005</t>
+  </si>
+  <si>
+    <t>TAG006</t>
+  </si>
+  <si>
+    <t>TAG007</t>
+  </si>
+  <si>
+    <t>TAG008</t>
+  </si>
+  <si>
+    <t>TAG009</t>
+  </si>
+  <si>
+    <t>TAG010</t>
+  </si>
+  <si>
+    <t>TAG011</t>
+  </si>
+  <si>
+    <t>TAG012</t>
+  </si>
+  <si>
+    <t>TAG013</t>
+  </si>
+  <si>
+    <t>TAG014</t>
+  </si>
+  <si>
+    <t>TAG015</t>
+  </si>
+  <si>
+    <t>TAG016</t>
+  </si>
+  <si>
+    <t>TAG017</t>
+  </si>
+  <si>
+    <t>TAG018</t>
+  </si>
+  <si>
+    <t>TAG019</t>
+  </si>
+  <si>
+    <t>TAG020</t>
+  </si>
+  <si>
+    <t>TAG021</t>
+  </si>
+  <si>
+    <t>TAG022</t>
+  </si>
+  <si>
+    <t>TAG023</t>
+  </si>
+  <si>
+    <t>TAG024</t>
+  </si>
+  <si>
+    <t>AA</t>
+  </si>
+  <si>
+    <t>BB</t>
+  </si>
+  <si>
+    <t>0001</t>
+  </si>
+  <si>
+    <t>DesignPressureUOM</t>
+  </si>
+  <si>
+    <t>PSI</t>
+  </si>
+  <si>
+    <t>DiffPressureUOM</t>
+  </si>
+  <si>
+    <t>NominalDiameter</t>
+  </si>
+  <si>
+    <t>NominalDiameterUOM</t>
+  </si>
+  <si>
+    <t>mm</t>
+  </si>
+  <si>
+    <t>KPA</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -576,8 +713,10 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -912,253 +1051,1086 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <x:dimension ref="A1:H9"/>
-  <x:sheetViews>
-    <x:sheetView tabSelected="1" workbookViewId="0">
-      <x:selection activeCell="A6" sqref="A6:XFD9"/>
-    </x:sheetView>
-  </x:sheetViews>
-  <x:sheetFormatPr defaultRowHeight="15"/>
-  <x:cols>
-    <x:col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
-  </x:cols>
-  <x:sheetData>
-    <x:row r="1" spans="1:8">
-      <x:c r="A1" t="s">
-        <x:v>4</x:v>
-      </x:c>
-      <x:c r="B1" t="s">
-        <x:v>5</x:v>
-      </x:c>
-      <x:c r="C1" t="s">
-        <x:v>6</x:v>
-      </x:c>
-      <x:c r="D1" t="s">
-        <x:v>7</x:v>
-      </x:c>
-      <x:c r="E1" t="s">
-        <x:v>8</x:v>
-      </x:c>
-      <x:c r="F1" t="s">
-        <x:v>9</x:v>
-      </x:c>
-      <x:c r="G1" t="s">
-        <x:v>10</x:v>
-      </x:c>
-      <x:c r="H1" t="s">
-        <x:v>11</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="2" spans="1:8">
-      <x:c r="A2" t="s">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="B2" t="s">
-        <x:v>12</x:v>
-      </x:c>
-      <x:c r="C2" t="s">
-        <x:v>15</x:v>
-      </x:c>
-      <x:c r="D2">
-        <x:v>7</x:v>
-      </x:c>
-      <x:c r="E2">
-        <x:v>8</x:v>
-      </x:c>
-      <x:c r="F2">
-        <x:v>9</x:v>
-      </x:c>
-      <x:c r="G2">
-        <x:v>3</x:v>
-      </x:c>
-      <x:c r="H2">
-        <x:v>7</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="3" spans="1:8">
-      <x:c r="A3" t="s">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="B3" t="s">
-        <x:v>12</x:v>
-      </x:c>
-      <x:c r="C3" t="s">
-        <x:v>13</x:v>
-      </x:c>
-      <x:c r="D3">
-        <x:v>2</x:v>
-      </x:c>
-      <x:c r="E3">
-        <x:v>3</x:v>
-      </x:c>
-      <x:c r="F3">
-        <x:v>7</x:v>
-      </x:c>
-      <x:c r="G3">
-        <x:v>8</x:v>
-      </x:c>
-      <x:c r="H3">
-        <x:v>9</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="4" spans="1:8">
-      <x:c r="A4" t="s">
-        <x:v>2</x:v>
-      </x:c>
-      <x:c r="B4" t="s">
-        <x:v>12</x:v>
-      </x:c>
-      <x:c r="C4" t="s">
-        <x:v>14</x:v>
-      </x:c>
-      <x:c r="D4">
-        <x:v>7</x:v>
-      </x:c>
-      <x:c r="E4">
-        <x:v>3</x:v>
-      </x:c>
-      <x:c r="F4">
-        <x:v>3</x:v>
-      </x:c>
-      <x:c r="G4">
-        <x:v>2</x:v>
-      </x:c>
-      <x:c r="H4">
-        <x:v>6</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="5" spans="1:8">
-      <x:c r="A5" t="s">
-        <x:v>3</x:v>
-      </x:c>
-      <x:c r="B5" t="s">
-        <x:v>12</x:v>
-      </x:c>
-      <x:c r="C5" t="s">
-        <x:v>14</x:v>
-      </x:c>
-      <x:c r="D5">
-        <x:v>7</x:v>
-      </x:c>
-      <x:c r="E5">
-        <x:v>3</x:v>
-      </x:c>
-      <x:c r="F5">
-        <x:v>3</x:v>
-      </x:c>
-      <x:c r="G5">
-        <x:v>2</x:v>
-      </x:c>
-      <x:c r="H5">
-        <x:v>6</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="6" spans="1:8">
-      <x:c r="A6" t="str">
-        <x:v>Equip-001</x:v>
-      </x:c>
-      <x:c r="B6" t="str">
-        <x:v>PT-8</x:v>
-      </x:c>
-      <x:c r="C6" t="str">
-        <x:v>PDT-5</x:v>
-      </x:c>
-      <x:c r="D6" t="str">
-        <x:v>9</x:v>
-      </x:c>
-      <x:c r="E6" t="str">
-        <x:v>6</x:v>
-      </x:c>
-      <x:c r="F6" t="str">
-        <x:v>7</x:v>
-      </x:c>
-      <x:c r="G6" t="str">
-        <x:v>7</x:v>
-      </x:c>
-      <x:c r="H6" t="str">
-        <x:v>3</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="7" spans="1:8">
-      <x:c r="A7" t="str">
-        <x:v>Equip-002</x:v>
-      </x:c>
-      <x:c r="B7" t="str">
-        <x:v>PT-7</x:v>
-      </x:c>
-      <x:c r="C7" t="str">
-        <x:v>PDT-9</x:v>
-      </x:c>
-      <x:c r="D7" t="str">
-        <x:v>6</x:v>
-      </x:c>
-      <x:c r="E7" t="str">
-        <x:v>2</x:v>
-      </x:c>
-      <x:c r="F7" t="str">
-        <x:v>5</x:v>
-      </x:c>
-      <x:c r="G7" t="str">
-        <x:v>7</x:v>
-      </x:c>
-      <x:c r="H7" t="str">
-        <x:v>7</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="8" spans="1:8">
-      <x:c r="A8" t="str">
-        <x:v>Equip-003</x:v>
-      </x:c>
-      <x:c r="B8" t="str">
-        <x:v>PT-3</x:v>
-      </x:c>
-      <x:c r="C8" t="str">
-        <x:v>PDT-6</x:v>
-      </x:c>
-      <x:c r="D8" t="str">
-        <x:v>7</x:v>
-      </x:c>
-      <x:c r="E8" t="str">
-        <x:v>3</x:v>
-      </x:c>
-      <x:c r="F8" t="str">
-        <x:v>5</x:v>
-      </x:c>
-      <x:c r="G8" t="str">
-        <x:v>4</x:v>
-      </x:c>
-      <x:c r="H8" t="str">
-        <x:v>5</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="9" spans="1:8">
-      <x:c r="A9" t="str">
-        <x:v>Equip-004</x:v>
-      </x:c>
-      <x:c r="B9" t="str">
-        <x:v>PT-6</x:v>
-      </x:c>
-      <x:c r="C9" t="str">
-        <x:v>PDT-4</x:v>
-      </x:c>
-      <x:c r="D9" t="str">
-        <x:v>2</x:v>
-      </x:c>
-      <x:c r="E9" t="str">
-        <x:v>7</x:v>
-      </x:c>
-      <x:c r="F9" t="str">
-        <x:v>4</x:v>
-      </x:c>
-      <x:c r="G9" t="str">
-        <x:v>4</x:v>
-      </x:c>
-      <x:c r="H9" t="str">
-        <x:v>6</x:v>
-      </x:c>
-    </x:row>
-  </x:sheetData>
-  <x:pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</x:worksheet>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:H9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2">
+        <v>7</v>
+      </c>
+      <c r="E2">
+        <v>8</v>
+      </c>
+      <c r="F2">
+        <v>9</v>
+      </c>
+      <c r="G2">
+        <v>3</v>
+      </c>
+      <c r="H2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+      <c r="E3">
+        <v>3</v>
+      </c>
+      <c r="F3">
+        <v>7</v>
+      </c>
+      <c r="G3">
+        <v>8</v>
+      </c>
+      <c r="H3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4">
+        <v>7</v>
+      </c>
+      <c r="E4">
+        <v>3</v>
+      </c>
+      <c r="F4">
+        <v>3</v>
+      </c>
+      <c r="G4">
+        <v>2</v>
+      </c>
+      <c r="H4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5">
+        <v>7</v>
+      </c>
+      <c r="E5">
+        <v>3</v>
+      </c>
+      <c r="F5">
+        <v>3</v>
+      </c>
+      <c r="G5">
+        <v>2</v>
+      </c>
+      <c r="H5">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" t="s">
+        <v>26</v>
+      </c>
+      <c r="F6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G6" t="s">
+        <v>27</v>
+      </c>
+      <c r="H6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F7" t="s">
+        <v>31</v>
+      </c>
+      <c r="G7" t="s">
+        <v>27</v>
+      </c>
+      <c r="H7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" t="s">
+        <v>27</v>
+      </c>
+      <c r="E8" t="s">
+        <v>28</v>
+      </c>
+      <c r="F8" t="s">
+        <v>31</v>
+      </c>
+      <c r="G8" t="s">
+        <v>32</v>
+      </c>
+      <c r="H8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" t="s">
+        <v>30</v>
+      </c>
+      <c r="E9" t="s">
+        <v>27</v>
+      </c>
+      <c r="F9" t="s">
+        <v>32</v>
+      </c>
+      <c r="G9" t="s">
+        <v>32</v>
+      </c>
+      <c r="H9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:K25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.5703125" customWidth="1"/>
+    <col min="4" max="4" width="16.140625" customWidth="1"/>
+    <col min="5" max="6" width="23.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11">
+      <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
+      <c r="A2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2">
+        <v>300</v>
+      </c>
+      <c r="C2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E2">
+        <v>50</v>
+      </c>
+      <c r="F2" t="s">
+        <v>65</v>
+      </c>
+      <c r="G2">
+        <v>15</v>
+      </c>
+      <c r="H2" t="s">
+        <v>69</v>
+      </c>
+      <c r="J2">
+        <v>22</v>
+      </c>
+      <c r="K2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
+      <c r="A3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3">
+        <v>300</v>
+      </c>
+      <c r="C3" t="s">
+        <v>61</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E3">
+        <v>50</v>
+      </c>
+      <c r="F3" t="s">
+        <v>65</v>
+      </c>
+      <c r="G3">
+        <v>15</v>
+      </c>
+      <c r="H3" t="s">
+        <v>69</v>
+      </c>
+      <c r="J3">
+        <v>22</v>
+      </c>
+      <c r="K3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="A4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4">
+        <v>300</v>
+      </c>
+      <c r="C4" t="s">
+        <v>61</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E4">
+        <v>50</v>
+      </c>
+      <c r="F4" t="s">
+        <v>65</v>
+      </c>
+      <c r="G4">
+        <v>15</v>
+      </c>
+      <c r="H4" t="s">
+        <v>69</v>
+      </c>
+      <c r="J4">
+        <v>22</v>
+      </c>
+      <c r="K4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="A5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B5">
+        <v>300</v>
+      </c>
+      <c r="C5" t="s">
+        <v>61</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E5">
+        <v>50</v>
+      </c>
+      <c r="F5" t="s">
+        <v>65</v>
+      </c>
+      <c r="G5">
+        <v>15</v>
+      </c>
+      <c r="H5" t="s">
+        <v>69</v>
+      </c>
+      <c r="J5">
+        <v>22</v>
+      </c>
+      <c r="K5" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="A6" t="s">
+        <v>41</v>
+      </c>
+      <c r="B6">
+        <v>300</v>
+      </c>
+      <c r="C6" t="s">
+        <v>61</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E6">
+        <v>50</v>
+      </c>
+      <c r="F6" t="s">
+        <v>65</v>
+      </c>
+      <c r="G6">
+        <v>15</v>
+      </c>
+      <c r="H6" t="s">
+        <v>69</v>
+      </c>
+      <c r="J6">
+        <v>22</v>
+      </c>
+      <c r="K6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="A7" t="s">
+        <v>42</v>
+      </c>
+      <c r="B7">
+        <v>300</v>
+      </c>
+      <c r="C7" t="s">
+        <v>61</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E7">
+        <v>50</v>
+      </c>
+      <c r="F7" t="s">
+        <v>65</v>
+      </c>
+      <c r="G7">
+        <v>15</v>
+      </c>
+      <c r="H7" t="s">
+        <v>69</v>
+      </c>
+      <c r="J7">
+        <v>22</v>
+      </c>
+      <c r="K7" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
+      <c r="A8" t="s">
+        <v>43</v>
+      </c>
+      <c r="B8">
+        <v>300</v>
+      </c>
+      <c r="C8" t="s">
+        <v>62</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E8">
+        <v>50</v>
+      </c>
+      <c r="F8" t="s">
+        <v>65</v>
+      </c>
+      <c r="G8">
+        <v>15</v>
+      </c>
+      <c r="H8" t="s">
+        <v>69</v>
+      </c>
+      <c r="J8">
+        <v>22</v>
+      </c>
+      <c r="K8" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
+      <c r="A9" t="s">
+        <v>44</v>
+      </c>
+      <c r="B9">
+        <v>300</v>
+      </c>
+      <c r="C9" t="s">
+        <v>62</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E9">
+        <v>50</v>
+      </c>
+      <c r="F9" t="s">
+        <v>65</v>
+      </c>
+      <c r="G9">
+        <v>15</v>
+      </c>
+      <c r="H9" t="s">
+        <v>69</v>
+      </c>
+      <c r="J9">
+        <v>22</v>
+      </c>
+      <c r="K9" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
+      <c r="A10" t="s">
+        <v>45</v>
+      </c>
+      <c r="B10">
+        <v>300</v>
+      </c>
+      <c r="C10" t="s">
+        <v>62</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E10">
+        <v>50</v>
+      </c>
+      <c r="F10" t="s">
+        <v>65</v>
+      </c>
+      <c r="G10">
+        <v>15</v>
+      </c>
+      <c r="H10" t="s">
+        <v>69</v>
+      </c>
+      <c r="J10">
+        <v>22</v>
+      </c>
+      <c r="K10" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
+      <c r="A11" t="s">
+        <v>46</v>
+      </c>
+      <c r="B11">
+        <v>300</v>
+      </c>
+      <c r="C11" t="s">
+        <v>62</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E11">
+        <v>50</v>
+      </c>
+      <c r="F11" t="s">
+        <v>65</v>
+      </c>
+      <c r="G11">
+        <v>15</v>
+      </c>
+      <c r="H11" t="s">
+        <v>69</v>
+      </c>
+      <c r="J11">
+        <v>22</v>
+      </c>
+      <c r="K11" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11">
+      <c r="A12" t="s">
+        <v>47</v>
+      </c>
+      <c r="B12">
+        <v>300</v>
+      </c>
+      <c r="C12" t="s">
+        <v>62</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E12">
+        <v>50</v>
+      </c>
+      <c r="F12" t="s">
+        <v>65</v>
+      </c>
+      <c r="G12">
+        <v>15</v>
+      </c>
+      <c r="H12" t="s">
+        <v>69</v>
+      </c>
+      <c r="J12">
+        <v>22</v>
+      </c>
+      <c r="K12" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11">
+      <c r="A13" t="s">
+        <v>48</v>
+      </c>
+      <c r="B13">
+        <v>300</v>
+      </c>
+      <c r="C13" t="s">
+        <v>62</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E13">
+        <v>50</v>
+      </c>
+      <c r="F13" t="s">
+        <v>65</v>
+      </c>
+      <c r="G13">
+        <v>15</v>
+      </c>
+      <c r="H13" t="s">
+        <v>69</v>
+      </c>
+      <c r="J13">
+        <v>22</v>
+      </c>
+      <c r="K13" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11">
+      <c r="A14" t="s">
+        <v>49</v>
+      </c>
+      <c r="B14">
+        <v>300</v>
+      </c>
+      <c r="C14" t="s">
+        <v>62</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E14">
+        <v>50</v>
+      </c>
+      <c r="F14" t="s">
+        <v>65</v>
+      </c>
+      <c r="G14">
+        <v>15</v>
+      </c>
+      <c r="H14" t="s">
+        <v>69</v>
+      </c>
+      <c r="J14">
+        <v>22</v>
+      </c>
+      <c r="K14" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11">
+      <c r="A15" t="s">
+        <v>50</v>
+      </c>
+      <c r="B15">
+        <v>400</v>
+      </c>
+      <c r="C15" t="s">
+        <v>61</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E15">
+        <v>2.4</v>
+      </c>
+      <c r="F15" t="s">
+        <v>70</v>
+      </c>
+      <c r="G15">
+        <v>40</v>
+      </c>
+      <c r="H15" t="s">
+        <v>69</v>
+      </c>
+      <c r="J15">
+        <v>22</v>
+      </c>
+      <c r="K15" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11">
+      <c r="A16" t="s">
+        <v>51</v>
+      </c>
+      <c r="B16">
+        <v>400</v>
+      </c>
+      <c r="C16" t="s">
+        <v>61</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E16">
+        <v>2.4</v>
+      </c>
+      <c r="F16" t="s">
+        <v>70</v>
+      </c>
+      <c r="G16">
+        <v>40</v>
+      </c>
+      <c r="H16" t="s">
+        <v>69</v>
+      </c>
+      <c r="J16">
+        <v>22</v>
+      </c>
+      <c r="K16" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11">
+      <c r="A17" t="s">
+        <v>52</v>
+      </c>
+      <c r="B17">
+        <v>400</v>
+      </c>
+      <c r="C17" t="s">
+        <v>61</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E17">
+        <v>2.4</v>
+      </c>
+      <c r="F17" t="s">
+        <v>70</v>
+      </c>
+      <c r="G17">
+        <v>40</v>
+      </c>
+      <c r="H17" t="s">
+        <v>69</v>
+      </c>
+      <c r="J17">
+        <v>22</v>
+      </c>
+      <c r="K17" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11">
+      <c r="A18" t="s">
+        <v>53</v>
+      </c>
+      <c r="B18">
+        <v>400</v>
+      </c>
+      <c r="C18" t="s">
+        <v>61</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E18">
+        <v>2.4</v>
+      </c>
+      <c r="F18" t="s">
+        <v>70</v>
+      </c>
+      <c r="G18">
+        <v>40</v>
+      </c>
+      <c r="H18" t="s">
+        <v>69</v>
+      </c>
+      <c r="J18">
+        <v>22</v>
+      </c>
+      <c r="K18" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11">
+      <c r="A19" t="s">
+        <v>54</v>
+      </c>
+      <c r="B19">
+        <v>400</v>
+      </c>
+      <c r="C19" t="s">
+        <v>61</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E19">
+        <v>2.4</v>
+      </c>
+      <c r="F19" t="s">
+        <v>70</v>
+      </c>
+      <c r="G19">
+        <v>40</v>
+      </c>
+      <c r="H19" t="s">
+        <v>69</v>
+      </c>
+      <c r="J19">
+        <v>22</v>
+      </c>
+      <c r="K19" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11">
+      <c r="A20" t="s">
+        <v>55</v>
+      </c>
+      <c r="B20">
+        <v>400</v>
+      </c>
+      <c r="C20" t="s">
+        <v>62</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E20">
+        <v>2.4</v>
+      </c>
+      <c r="F20" t="s">
+        <v>70</v>
+      </c>
+      <c r="G20">
+        <v>40</v>
+      </c>
+      <c r="H20" t="s">
+        <v>69</v>
+      </c>
+      <c r="J20">
+        <v>22</v>
+      </c>
+      <c r="K20" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11">
+      <c r="A21" t="s">
+        <v>56</v>
+      </c>
+      <c r="B21">
+        <v>400</v>
+      </c>
+      <c r="C21" t="s">
+        <v>62</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E21">
+        <v>2.4</v>
+      </c>
+      <c r="F21" t="s">
+        <v>70</v>
+      </c>
+      <c r="G21">
+        <v>40</v>
+      </c>
+      <c r="H21" t="s">
+        <v>69</v>
+      </c>
+      <c r="J21">
+        <v>22</v>
+      </c>
+      <c r="K21" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11">
+      <c r="A22" t="s">
+        <v>57</v>
+      </c>
+      <c r="B22">
+        <v>400</v>
+      </c>
+      <c r="C22" t="s">
+        <v>62</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E22">
+        <v>2.4</v>
+      </c>
+      <c r="F22" t="s">
+        <v>70</v>
+      </c>
+      <c r="G22">
+        <v>40</v>
+      </c>
+      <c r="H22" t="s">
+        <v>69</v>
+      </c>
+      <c r="J22">
+        <v>22</v>
+      </c>
+      <c r="K22" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11">
+      <c r="A23" t="s">
+        <v>58</v>
+      </c>
+      <c r="B23">
+        <v>400</v>
+      </c>
+      <c r="C23" t="s">
+        <v>62</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E23">
+        <v>2.4</v>
+      </c>
+      <c r="F23" t="s">
+        <v>70</v>
+      </c>
+      <c r="G23">
+        <v>40</v>
+      </c>
+      <c r="H23" t="s">
+        <v>69</v>
+      </c>
+      <c r="J23">
+        <v>22</v>
+      </c>
+      <c r="K23" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11">
+      <c r="A24" t="s">
+        <v>59</v>
+      </c>
+      <c r="B24">
+        <v>400</v>
+      </c>
+      <c r="C24" t="s">
+        <v>62</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E24">
+        <v>2.4</v>
+      </c>
+      <c r="F24" t="s">
+        <v>70</v>
+      </c>
+      <c r="G24">
+        <v>40</v>
+      </c>
+      <c r="H24" t="s">
+        <v>69</v>
+      </c>
+      <c r="J24">
+        <v>22</v>
+      </c>
+      <c r="K24" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11">
+      <c r="A25" t="s">
+        <v>60</v>
+      </c>
+      <c r="B25">
+        <v>400</v>
+      </c>
+      <c r="C25" t="s">
+        <v>62</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E25">
+        <v>2.4</v>
+      </c>
+      <c r="F25" t="s">
+        <v>70</v>
+      </c>
+      <c r="G25">
+        <v>40</v>
+      </c>
+      <c r="H25" t="s">
+        <v>69</v>
+      </c>
+      <c r="J25">
+        <v>22</v>
+      </c>
+      <c r="K25" t="s">
+        <v>65</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>